<commit_message>
Add new songs to playlist and update selected video ID; refine animation triggers for song and author changes
</commit_message>
<xml_diff>
--- a/resource/files/playlist.xlsx
+++ b/resource/files/playlist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\YouTube-Music-Player-Web\resource\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8874F593-C3BE-46C4-8A4D-C4B4B1B0E2B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19C8E45-F506-4860-B271-27713CF0AD53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="103">
   <si>
     <t>Song Name</t>
   </si>
@@ -305,6 +305,30 @@
   </si>
   <si>
     <t>TQ8WlA2GXbk</t>
+  </si>
+  <si>
+    <t>無名的人</t>
+  </si>
+  <si>
+    <t>贝加尔湖畔</t>
+  </si>
+  <si>
+    <t>风吹麦浪</t>
+  </si>
+  <si>
+    <t>毛不易</t>
+  </si>
+  <si>
+    <t>李健</t>
+  </si>
+  <si>
+    <t>LgNT-a_ekC8</t>
+  </si>
+  <si>
+    <t>Oewc0KgfQUU</t>
+  </si>
+  <si>
+    <t>Nk9ztUjikT0</t>
   </si>
 </sst>
 </file>
@@ -363,11 +387,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -672,15 +698,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -691,366 +717,402 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B7" t="s">
         <v>31</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>89</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B8" t="s">
         <v>88</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C8" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>91</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B9" t="s">
         <v>88</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C9" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>90</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B10" t="s">
         <v>88</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C10" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B11" t="s">
         <v>32</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B12" t="s">
         <v>32</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C12" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B13" t="s">
         <v>33</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B14" t="s">
         <v>34</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C14" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B15" t="s">
         <v>35</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C15" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B16" t="s">
         <v>36</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C16" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C21" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C22" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C26" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C27" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C28" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B29" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C29" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>82</v>
+        <v>23</v>
       </c>
       <c r="B30" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="C30" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>87</v>
+        <v>24</v>
       </c>
       <c r="B31" t="s">
-        <v>86</v>
+        <v>47</v>
       </c>
       <c r="C31" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B32" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C32" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>82</v>
       </c>
       <c r="B33" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="C33" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>30</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B37" t="s">
         <v>53</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C37" t="s">
         <v>81</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add new songs to playlist
</commit_message>
<xml_diff>
--- a/resource/files/playlist.xlsx
+++ b/resource/files/playlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\YouTube-Music-Player-Web\resource\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19C8E45-F506-4860-B271-27713CF0AD53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB363595-CEBD-4622-AD9F-2F00362E34B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="106">
   <si>
     <t>Song Name</t>
   </si>
@@ -307,9 +307,6 @@
     <t>TQ8WlA2GXbk</t>
   </si>
   <si>
-    <t>無名的人</t>
-  </si>
-  <si>
     <t>贝加尔湖畔</t>
   </si>
   <si>
@@ -329,6 +326,18 @@
   </si>
   <si>
     <t>Nk9ztUjikT0</t>
+  </si>
+  <si>
+    <t>无名的人</t>
+  </si>
+  <si>
+    <t>点燃银河尽头的篝火</t>
+  </si>
+  <si>
+    <t>华晨宇</t>
+  </si>
+  <si>
+    <t>yBaYm7Ig7ZQ</t>
   </si>
 </sst>
 </file>
@@ -387,13 +396,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -698,15 +705,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -717,402 +724,410 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B4" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C4" t="s">
         <v>100</v>
       </c>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" t="s">
         <v>101</v>
       </c>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>26</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>49</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>27</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>50</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>3</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>31</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>89</v>
-      </c>
-      <c r="B8" t="s">
-        <v>88</v>
-      </c>
-      <c r="C8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>91</v>
       </c>
       <c r="B9" t="s">
         <v>88</v>
       </c>
       <c r="C9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B10" t="s">
         <v>88</v>
       </c>
       <c r="C10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>5</v>
       </c>
       <c r="B12" t="s">
         <v>32</v>
       </c>
       <c r="C12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>6</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>33</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>7</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>34</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>8</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>35</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19" t="s">
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
         <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B21" t="s">
         <v>38</v>
       </c>
       <c r="C21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B22" t="s">
         <v>38</v>
       </c>
       <c r="C22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>82</v>
+        <v>25</v>
       </c>
       <c r="B33" t="s">
-        <v>83</v>
+        <v>48</v>
       </c>
       <c r="C33" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B34" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>28</v>
+        <v>87</v>
       </c>
       <c r="B35" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
       <c r="C35" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>30</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>53</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>81</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add new songs to playlist and update playlist file
</commit_message>
<xml_diff>
--- a/resource/files/playlist.xlsx
+++ b/resource/files/playlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\YouTube-Music-Player-Web\resource\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB363595-CEBD-4622-AD9F-2F00362E34B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A508786D-C7D3-40FC-8B38-8F51CE4B89C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="112">
   <si>
     <t>Song Name</t>
   </si>
@@ -338,6 +338,24 @@
   </si>
   <si>
     <t>yBaYm7Ig7ZQ</t>
+  </si>
+  <si>
+    <t>回不去的夏天</t>
+  </si>
+  <si>
+    <t>夏日入侵企画</t>
+  </si>
+  <si>
+    <t>mrY8qdNHcRs</t>
+  </si>
+  <si>
+    <t>我們都擁有海洋 (嗶哩嗶哩2023畢業歌)</t>
+  </si>
+  <si>
+    <t>吳青峰</t>
+  </si>
+  <si>
+    <t>rQOIRBrY7h0</t>
   </si>
 </sst>
 </file>
@@ -705,10 +723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -792,342 +810,364 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="C9" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>92</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B11" t="s">
         <v>88</v>
       </c>
       <c r="C11" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>91</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>88</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>90</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>88</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B21" t="s">
         <v>38</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B22" t="s">
         <v>38</v>
       </c>
       <c r="C22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B23" t="s">
         <v>38</v>
       </c>
       <c r="C23" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C24" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C27" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B29" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C30" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B31" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C31" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B32" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C32" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B33" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C33" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>82</v>
+        <v>24</v>
       </c>
       <c r="B34" t="s">
-        <v>83</v>
+        <v>47</v>
       </c>
       <c r="C34" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>87</v>
+        <v>25</v>
       </c>
       <c r="B35" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="C35" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="B36" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="C36" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="B37" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="C37" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>30</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B40" t="s">
         <v>53</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C40" t="s">
         <v>81</v>
       </c>
     </row>

</xml_diff>